<commit_message>
Update to support both R4B and R5.
Code will need clean up after testing both implementations for R4B and R5. Structure has changed under services package
</commit_message>
<xml_diff>
--- a/resources/SubtancesCodeTemplate_RVS_V5.xlsx
+++ b/resources/SubtancesCodeTemplate_RVS_V5.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ugentbe-my.sharepoint.com/personal/robert_vanderstichele_ugent_be/Documents/Documents/UNICOM/PPLSubprojects/resouruces/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brion\Documents\UNICOM\deliverables\6.6\GitHub\wp6-NCPeH-substitution\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{7C81D52D-A8CA-46C9-A444-49F2FA78DABC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{954F3B98-28F9-4347-A9C8-114C8D5DD1E0}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64A1697E-8DB3-4028-8E5A-5B07F9420B8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{EB1B301A-6B6A-4CBE-BDF5-B3082E408CF9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="3" xr2:uid="{EB1B301A-6B6A-4CBE-BDF5-B3082E408CF9}"/>
   </bookViews>
   <sheets>
     <sheet name="full codes" sheetId="1" r:id="rId1"/>
@@ -3176,7 +3176,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3217,7 +3217,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -3515,27 +3515,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA6896D3-C0DA-4B89-A0FE-FB94E33A1A9A}">
   <dimension ref="A1:R114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="R8" sqref="R8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.5546875" customWidth="1"/>
-    <col min="2" max="2" width="4.88671875" customWidth="1"/>
-    <col min="3" max="4" width="17.44140625" customWidth="1"/>
+    <col min="1" max="1" width="30.5703125" customWidth="1"/>
+    <col min="2" max="2" width="4.85546875" customWidth="1"/>
+    <col min="3" max="4" width="17.42578125" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="31.77734375" customWidth="1"/>
-    <col min="11" max="11" width="14.6640625" customWidth="1"/>
-    <col min="15" max="15" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="31.7109375" customWidth="1"/>
+    <col min="11" max="11" width="14.7109375" customWidth="1"/>
+    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="20" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="15" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="22.21875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="22.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="21"/>
       <c r="B1" s="21" t="s">
         <v>154</v>
@@ -3573,7 +3573,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>79</v>
       </c>
@@ -3584,7 +3584,7 @@
       <c r="Q2" s="84"/>
       <c r="R2" s="84"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -3619,7 +3619,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>45</v>
       </c>
@@ -3654,7 +3654,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>0</v>
       </c>
@@ -3691,7 +3691,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>66</v>
       </c>
@@ -3726,7 +3726,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
         <v>80</v>
       </c>
@@ -3763,7 +3763,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>85</v>
       </c>
@@ -3797,7 +3797,7 @@
         <v>BEL amlodipine besylate Aurobindo tablet 100 x 10mg/</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>136</v>
       </c>
@@ -3830,7 +3830,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
         <v>105</v>
       </c>
@@ -3868,7 +3868,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="43" t="s">
         <v>122</v>
       </c>
@@ -3903,7 +3903,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="19" t="s">
         <v>152</v>
       </c>
@@ -3937,7 +3937,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="47" t="s">
         <v>138</v>
       </c>
@@ -3974,7 +3974,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="43" t="s">
         <v>153</v>
       </c>
@@ -4008,7 +4008,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>156</v>
       </c>
@@ -4044,7 +4044,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="37" t="s">
         <v>176</v>
       </c>
@@ -4080,7 +4080,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>175</v>
       </c>
@@ -4116,7 +4116,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="37" t="s">
         <v>174</v>
       </c>
@@ -4152,7 +4152,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="19" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="50" t="s">
         <v>173</v>
       </c>
@@ -4188,7 +4188,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="20" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="50" t="s">
         <v>181</v>
       </c>
@@ -4224,7 +4224,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="21" spans="1:18" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:18" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="18" t="s">
         <v>199</v>
       </c>
@@ -4260,7 +4260,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="22" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="71" t="s">
         <v>224</v>
       </c>
@@ -4294,7 +4294,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="18" t="s">
         <v>233</v>
       </c>
@@ -4330,7 +4330,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="24" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="57" t="s">
         <v>279</v>
       </c>
@@ -4366,7 +4366,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="18" t="s">
         <v>289</v>
       </c>
@@ -4402,7 +4402,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="26" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="57" t="s">
         <v>301</v>
       </c>
@@ -4437,7 +4437,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="27" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="57" t="s">
         <v>312</v>
       </c>
@@ -4473,7 +4473,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="18" t="s">
         <v>325</v>
       </c>
@@ -4509,7 +4509,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="18" t="s">
         <v>340</v>
       </c>
@@ -4545,7 +4545,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="30" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="57" t="s">
         <v>360</v>
       </c>
@@ -4581,7 +4581,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="31" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="50" t="s">
         <v>373</v>
       </c>
@@ -4619,7 +4619,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="32" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="57" t="s">
         <v>375</v>
       </c>
@@ -4659,7 +4659,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="33" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="57" t="s">
         <v>386</v>
       </c>
@@ -4695,7 +4695,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="34" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="63" t="s">
         <v>391</v>
       </c>
@@ -4733,7 +4733,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35" s="18" t="s">
         <v>397</v>
       </c>
@@ -4769,7 +4769,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36" s="61" t="s">
         <v>421</v>
       </c>
@@ -4807,7 +4807,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37" s="46" t="s">
         <v>429</v>
       </c>
@@ -4843,7 +4843,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>442</v>
       </c>
@@ -4876,7 +4876,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" s="61" t="s">
         <v>464</v>
       </c>
@@ -4914,7 +4914,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40" s="3"/>
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
@@ -4925,7 +4925,7 @@
       <c r="H40" s="3"/>
       <c r="I40" s="4"/>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41" s="18"/>
       <c r="B41" s="18"/>
       <c r="C41" s="18"/>
@@ -4936,7 +4936,7 @@
       <c r="H41" s="3"/>
       <c r="I41" s="4"/>
     </row>
-    <row r="42" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="10" t="s">
         <v>71</v>
       </c>
@@ -4949,7 +4949,7 @@
       <c r="H42" s="3"/>
       <c r="I42" s="4"/>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43" s="59" t="s">
         <v>78</v>
       </c>
@@ -4972,7 +4972,7 @@
       </c>
       <c r="I43" s="4"/>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
         <v>9</v>
       </c>
@@ -4994,7 +4994,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45" s="9" t="s">
         <v>11</v>
       </c>
@@ -5016,7 +5016,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A46" s="9" t="s">
         <v>77</v>
       </c>
@@ -5039,7 +5039,7 @@
       </c>
       <c r="I46" s="19"/>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A47" s="9" t="s">
         <v>14</v>
       </c>
@@ -5061,7 +5061,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A48" s="9" t="s">
         <v>16</v>
       </c>
@@ -5083,7 +5083,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="9" t="s">
         <v>18</v>
       </c>
@@ -5105,7 +5105,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="17" t="s">
         <v>65</v>
       </c>
@@ -5127,7 +5127,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="20" t="s">
         <v>21</v>
       </c>
@@ -5149,7 +5149,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="20" t="s">
         <v>23</v>
       </c>
@@ -5171,7 +5171,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="9" t="s">
         <v>56</v>
       </c>
@@ -5193,7 +5193,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="54" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="24" t="s">
         <v>25</v>
       </c>
@@ -5217,7 +5217,7 @@
       <c r="I54" s="21"/>
       <c r="J54" s="21"/>
     </row>
-    <row r="55" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>80</v>
       </c>
@@ -5237,7 +5237,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="19" t="s">
         <v>90</v>
       </c>
@@ -5259,7 +5259,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="34" t="s">
         <v>95</v>
       </c>
@@ -5281,7 +5281,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="19" t="s">
         <v>101</v>
       </c>
@@ -5303,7 +5303,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
         <v>187</v>
       </c>
@@ -5325,7 +5325,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>193</v>
       </c>
@@ -5347,7 +5347,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="38" t="s">
         <v>110</v>
       </c>
@@ -5369,7 +5369,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="41" t="s">
         <v>116</v>
       </c>
@@ -5392,7 +5392,7 @@
       </c>
       <c r="K62" s="3"/>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>126</v>
       </c>
@@ -5413,7 +5413,7 @@
       </c>
       <c r="K63" s="3"/>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
         <v>142</v>
       </c>
@@ -5435,7 +5435,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="65" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A65" s="47" t="s">
         <v>138</v>
       </c>
@@ -5458,7 +5458,7 @@
       </c>
       <c r="I65" s="4"/>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66" s="38" t="s">
         <v>148</v>
       </c>
@@ -5480,7 +5480,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
         <v>175</v>
       </c>
@@ -5500,7 +5500,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68" s="37" t="s">
         <v>174</v>
       </c>
@@ -5520,7 +5520,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="69" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A69" s="50" t="s">
         <v>173</v>
       </c>
@@ -5540,7 +5540,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="70" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A70" s="50" t="s">
         <v>181</v>
       </c>
@@ -5560,7 +5560,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
         <v>206</v>
       </c>
@@ -5582,7 +5582,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
         <v>211</v>
       </c>
@@ -5604,7 +5604,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
         <v>216</v>
       </c>
@@ -5626,7 +5626,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
         <v>221</v>
       </c>
@@ -5648,7 +5648,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A75" s="37" t="s">
         <v>228</v>
       </c>
@@ -5675,7 +5675,7 @@
       <c r="L75" s="3"/>
       <c r="M75" s="3"/>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
         <v>234</v>
       </c>
@@ -5697,7 +5697,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
         <v>239</v>
       </c>
@@ -5719,7 +5719,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
         <v>244</v>
       </c>
@@ -5741,7 +5741,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
         <v>249</v>
       </c>
@@ -5763,7 +5763,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
         <v>254</v>
       </c>
@@ -5785,7 +5785,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
         <v>259</v>
       </c>
@@ -5807,7 +5807,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
         <v>264</v>
       </c>
@@ -5829,7 +5829,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
         <v>269</v>
       </c>
@@ -5851,7 +5851,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
         <v>280</v>
       </c>
@@ -5873,7 +5873,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="85" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A85" s="57" t="s">
         <v>290</v>
       </c>
@@ -5895,7 +5895,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
         <v>295</v>
       </c>
@@ -5917,7 +5917,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="87" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A87" s="50" t="s">
         <v>306</v>
       </c>
@@ -5939,7 +5939,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="88" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A88" s="50" t="s">
         <v>316</v>
       </c>
@@ -5961,7 +5961,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
         <v>326</v>
       </c>
@@ -5983,7 +5983,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="37" t="s">
         <v>331</v>
       </c>
@@ -6005,7 +6005,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
         <v>341</v>
       </c>
@@ -6027,7 +6027,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
         <v>346</v>
       </c>
@@ -6049,7 +6049,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
         <v>351</v>
       </c>
@@ -6071,7 +6071,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="3" t="s">
         <v>354</v>
       </c>
@@ -6093,7 +6093,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="95" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A95" s="50" t="s">
         <v>368</v>
       </c>
@@ -6115,7 +6115,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="96" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A96" s="50" t="s">
         <v>373</v>
       </c>
@@ -6137,7 +6137,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="97" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A97" s="57" t="s">
         <v>375</v>
       </c>
@@ -6162,7 +6162,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="98" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A98" s="50" t="s">
         <v>380</v>
       </c>
@@ -6184,7 +6184,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="99" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A99" s="63" t="s">
         <v>391</v>
       </c>
@@ -6206,7 +6206,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="s">
         <v>401</v>
       </c>
@@ -6228,7 +6228,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
         <v>406</v>
       </c>
@@ -6250,7 +6250,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" s="37" t="s">
         <v>411</v>
       </c>
@@ -6272,7 +6272,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" s="37" t="s">
         <v>416</v>
       </c>
@@ -6294,7 +6294,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" s="61" t="s">
         <v>421</v>
       </c>
@@ -6316,7 +6316,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" s="3" t="s">
         <v>438</v>
       </c>
@@ -6336,7 +6336,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" s="37" t="s">
         <v>468</v>
       </c>
@@ -6356,7 +6356,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" s="3" t="s">
         <v>443</v>
       </c>
@@ -6378,7 +6378,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108" s="37" t="s">
         <v>447</v>
       </c>
@@ -6401,7 +6401,7 @@
       </c>
       <c r="I108" s="37"/>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" s="70" t="s">
         <v>451</v>
       </c>
@@ -6419,7 +6419,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110" s="70" t="s">
         <v>454</v>
       </c>
@@ -6439,7 +6439,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111" s="70" t="s">
         <v>456</v>
       </c>
@@ -6461,7 +6461,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112" s="70" t="s">
         <v>457</v>
       </c>
@@ -6483,7 +6483,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" s="70" t="s">
         <v>460</v>
       </c>
@@ -6505,7 +6505,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" s="61" t="s">
         <v>464</v>
       </c>
@@ -6548,15 +6548,15 @@
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="30.5546875" customWidth="1"/>
+    <col min="2" max="2" width="30.5703125" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
-    <col min="4" max="4" width="4.88671875" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" customWidth="1"/>
+    <col min="4" max="4" width="4.85546875" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>515</v>
       </c>
@@ -6570,14 +6570,14 @@
       <c r="E1" s="23"/>
       <c r="F1" s="23"/>
     </row>
-    <row r="2" spans="1:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B2" s="11" t="s">
         <v>79</v>
       </c>
       <c r="C2" s="76"/>
       <c r="D2" s="11"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -6590,7 +6590,7 @@
       <c r="D3" s="3"/>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <f>A3+1</f>
         <v>2</v>
@@ -6604,7 +6604,7 @@
       <c r="D4" s="3"/>
       <c r="E4" s="4"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" ref="A5:A39" si="0">A4+1</f>
         <v>3</v>
@@ -6620,7 +6620,7 @@
       </c>
       <c r="E5" s="4"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -6634,7 +6634,7 @@
       <c r="D6" s="18"/>
       <c r="E6" s="4"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -6650,7 +6650,7 @@
       </c>
       <c r="E7" s="4"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -6663,7 +6663,7 @@
       </c>
       <c r="E8" s="4"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -6676,7 +6676,7 @@
       </c>
       <c r="E9" s="4"/>
     </row>
-    <row r="10" spans="1:7" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -6690,7 +6690,7 @@
       <c r="D10" s="18"/>
       <c r="E10" s="4"/>
     </row>
-    <row r="11" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -6704,7 +6704,7 @@
       <c r="D11" s="47"/>
       <c r="G11" s="45"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -6717,7 +6717,7 @@
       </c>
       <c r="D12" s="19"/>
     </row>
-    <row r="13" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -6733,7 +6733,7 @@
       </c>
       <c r="E13" s="4"/>
     </row>
-    <row r="14" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -6746,7 +6746,7 @@
       </c>
       <c r="D14" s="47"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -6762,7 +6762,7 @@
       </c>
       <c r="E15" s="4"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -6778,7 +6778,7 @@
       </c>
       <c r="E16" s="4"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -6794,7 +6794,7 @@
       </c>
       <c r="E17" s="4"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -6810,7 +6810,7 @@
       </c>
       <c r="E18" s="4"/>
     </row>
-    <row r="19" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -6826,7 +6826,7 @@
       </c>
       <c r="E19" s="4"/>
     </row>
-    <row r="20" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -6842,7 +6842,7 @@
       </c>
       <c r="E20" s="4"/>
     </row>
-    <row r="21" spans="1:6" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -6857,7 +6857,7 @@
       <c r="E21" s="3"/>
       <c r="F21" s="4"/>
     </row>
-    <row r="22" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -6870,7 +6870,7 @@
       </c>
       <c r="D22" s="71"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -6885,7 +6885,7 @@
       <c r="E23" s="3"/>
       <c r="F23" s="4"/>
     </row>
-    <row r="24" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -6900,7 +6900,7 @@
       <c r="E24" s="3"/>
       <c r="F24" s="4"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -6915,7 +6915,7 @@
       <c r="E25" s="3"/>
       <c r="F25" s="4"/>
     </row>
-    <row r="26" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -6929,7 +6929,7 @@
       <c r="D26" s="57"/>
       <c r="E26" s="4"/>
     </row>
-    <row r="27" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -6944,7 +6944,7 @@
       <c r="E27" s="3"/>
       <c r="F27" s="4"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -6959,7 +6959,7 @@
       <c r="E28" s="3"/>
       <c r="F28" s="4"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -6974,7 +6974,7 @@
       <c r="E29" s="3"/>
       <c r="F29" s="4"/>
     </row>
-    <row r="30" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -6989,7 +6989,7 @@
       <c r="E30" s="3"/>
       <c r="F30" s="4"/>
     </row>
-    <row r="31" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -7006,7 +7006,7 @@
       <c r="E31" s="3"/>
       <c r="F31" s="4"/>
     </row>
-    <row r="32" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -7023,7 +7023,7 @@
       <c r="E32" s="3"/>
       <c r="F32" s="62"/>
     </row>
-    <row r="33" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -7038,7 +7038,7 @@
       <c r="E33" s="3"/>
       <c r="F33" s="4"/>
     </row>
-    <row r="34" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -7055,7 +7055,7 @@
       <c r="E34" s="3"/>
       <c r="F34" s="4"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -7070,7 +7070,7 @@
       <c r="E35" s="3"/>
       <c r="F35" s="4"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -7087,7 +7087,7 @@
       <c r="E36" s="3"/>
       <c r="F36" s="4"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -7102,7 +7102,7 @@
       <c r="E37" s="3"/>
       <c r="F37" s="4"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -7115,7 +7115,7 @@
       </c>
       <c r="F38" s="3"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -7132,7 +7132,7 @@
       <c r="E39" s="3"/>
       <c r="F39" s="4"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B40" s="3"/>
       <c r="C40" s="36"/>
       <c r="D40" s="5"/>
@@ -7153,24 +7153,24 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.5546875" customWidth="1"/>
-    <col min="2" max="2" width="21.88671875" customWidth="1"/>
+    <col min="1" max="1" width="23.5703125" customWidth="1"/>
+    <col min="2" max="2" width="21.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>524</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="86" t="s">
         <v>516</v>
       </c>
       <c r="B5" s="85"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>9</v>
       </c>
@@ -7178,7 +7178,7 @@
         <v>100000092272</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>11</v>
       </c>
@@ -7186,7 +7186,7 @@
         <v>100000092368</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>478</v>
       </c>
@@ -7194,7 +7194,7 @@
         <v>100000091074</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>14</v>
       </c>
@@ -7202,7 +7202,7 @@
         <v>100000085789</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>16</v>
       </c>
@@ -7210,7 +7210,7 @@
         <v>100000090113</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>18</v>
       </c>
@@ -7218,11 +7218,11 @@
         <v>100000092629</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="9"/>
       <c r="B12" s="27"/>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
         <v>21</v>
       </c>
@@ -7230,7 +7230,7 @@
         <v>100000090079</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="20" t="s">
         <v>23</v>
       </c>
@@ -7238,7 +7238,7 @@
         <v>100000089571</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>25</v>
       </c>
@@ -7246,7 +7246,7 @@
         <v>100000089370</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="19" t="s">
         <v>90</v>
       </c>
@@ -7254,7 +7254,7 @@
         <v>100000091343</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="34" t="s">
         <v>95</v>
       </c>
@@ -7262,7 +7262,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="19" t="s">
         <v>101</v>
       </c>
@@ -7270,7 +7270,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>187</v>
       </c>
@@ -7278,7 +7278,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>193</v>
       </c>
@@ -7286,7 +7286,7 @@
         <v>100000085918</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="38" t="s">
         <v>110</v>
       </c>
@@ -7294,7 +7294,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="41" t="s">
         <v>116</v>
       </c>
@@ -7302,7 +7302,7 @@
         <v>100000093039</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>126</v>
       </c>
@@ -7310,7 +7310,7 @@
         <v>100000090564</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>142</v>
       </c>
@@ -7318,7 +7318,7 @@
         <v>100000093061</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="38" t="s">
         <v>148</v>
       </c>
@@ -7326,7 +7326,7 @@
         <v>100000084795</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>206</v>
       </c>
@@ -7334,7 +7334,7 @@
         <v>100000090494</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>211</v>
       </c>
@@ -7342,7 +7342,7 @@
         <v>100000076239</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>216</v>
       </c>
@@ -7350,7 +7350,7 @@
         <v>100000076257</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="37" t="s">
         <v>228</v>
       </c>
@@ -7358,7 +7358,7 @@
         <v>100000090152</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>234</v>
       </c>
@@ -7366,7 +7366,7 @@
         <v>100000092550</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>239</v>
       </c>
@@ -7374,7 +7374,7 @@
         <v>100000086711</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>244</v>
       </c>
@@ -7382,7 +7382,7 @@
         <v>100000092260</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>249</v>
       </c>
@@ -7390,7 +7390,7 @@
         <v>100000085172</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>254</v>
       </c>
@@ -7398,7 +7398,7 @@
         <v>100000084215</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>479</v>
       </c>
@@ -7406,7 +7406,7 @@
         <v>100000085172</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>264</v>
       </c>
@@ -7414,7 +7414,7 @@
         <v>100000086187</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>269</v>
       </c>
@@ -7422,7 +7422,7 @@
         <v>100000086691</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>280</v>
       </c>
@@ -7430,7 +7430,7 @@
         <v>100000139489</v>
       </c>
     </row>
-    <row r="47" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="57" t="s">
         <v>480</v>
       </c>
@@ -7438,7 +7438,7 @@
         <v>100000128434</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>295</v>
       </c>
@@ -7446,11 +7446,11 @@
         <v>100000174462</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="84"/>
       <c r="B49" s="84"/>
     </row>
-    <row r="50" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="50" t="s">
         <v>316</v>
       </c>
@@ -7458,7 +7458,7 @@
         <v>100000090503</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>326</v>
       </c>
@@ -7466,7 +7466,7 @@
         <v>100000091366</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="37" t="s">
         <v>483</v>
       </c>
@@ -7474,7 +7474,7 @@
         <v>100000091840</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>341</v>
       </c>
@@ -7482,7 +7482,7 @@
         <v>100000088816</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>484</v>
       </c>
@@ -7490,7 +7490,7 @@
         <v>100000091602</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>351</v>
       </c>
@@ -7498,7 +7498,7 @@
         <v>100000130680</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>354</v>
       </c>
@@ -7506,7 +7506,7 @@
         <v>100000141420</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" s="50" t="s">
         <v>368</v>
       </c>
@@ -7514,7 +7514,7 @@
         <v>100000093275</v>
       </c>
     </row>
-    <row r="60" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A60" s="50" t="s">
         <v>380</v>
       </c>
@@ -7522,7 +7522,7 @@
         <v>100000086673</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
         <v>401</v>
       </c>
@@ -7530,7 +7530,7 @@
         <v>100000092628</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
         <v>406</v>
       </c>
@@ -7538,7 +7538,7 @@
         <v>100000090551</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="37" t="s">
         <v>411</v>
       </c>
@@ -7546,7 +7546,7 @@
         <v>100000084735</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="37" t="s">
         <v>416</v>
       </c>
@@ -7554,7 +7554,7 @@
         <v>100000129152</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
         <v>438</v>
       </c>
@@ -7562,7 +7562,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="37" t="s">
         <v>468</v>
       </c>
@@ -7570,7 +7570,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
         <v>443</v>
       </c>
@@ -7578,7 +7578,7 @@
         <v>100000085009</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="37" t="s">
         <v>447</v>
       </c>
@@ -7586,7 +7586,7 @@
         <v>100000090111</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="61" t="s">
         <v>464</v>
       </c>
@@ -7604,28 +7604,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CA1A98B-F8D0-4016-8596-4D3002645926}">
   <dimension ref="A1:I143"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O14" sqref="O14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.77734375" customWidth="1"/>
-    <col min="2" max="3" width="15.44140625" customWidth="1"/>
-    <col min="4" max="4" width="30.21875" customWidth="1"/>
+    <col min="1" max="1" width="5.7109375" customWidth="1"/>
+    <col min="2" max="3" width="15.42578125" customWidth="1"/>
+    <col min="4" max="4" width="30.28515625" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
-    <col min="6" max="6" width="19.6640625" customWidth="1"/>
-    <col min="7" max="7" width="16.5546875" customWidth="1"/>
-    <col min="8" max="8" width="21.88671875" customWidth="1"/>
-    <col min="9" max="9" width="14.21875" customWidth="1"/>
+    <col min="6" max="6" width="19.7109375" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" customWidth="1"/>
+    <col min="8" max="8" width="21.85546875" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="89" t="s">
         <v>519</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="11"/>
       <c r="B4" s="11" t="s">
         <v>525</v>
@@ -7643,7 +7643,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="85" customFormat="1" ht="42" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" s="85" customFormat="1" ht="39.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>515</v>
       </c>
@@ -7662,7 +7662,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
@@ -7691,7 +7691,7 @@
         <v>100000092272</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D7" s="9" t="s">
         <v>11</v>
       </c>
@@ -7711,7 +7711,7 @@
         <v>100000092368</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D8" s="9" t="s">
         <v>478</v>
       </c>
@@ -7731,7 +7731,7 @@
         <v>100000091074</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D9" s="9" t="s">
         <v>14</v>
       </c>
@@ -7751,7 +7751,7 @@
         <v>100000085789</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2</v>
       </c>
@@ -7780,7 +7780,7 @@
         <v>100000090113</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D11" s="9" t="s">
         <v>18</v>
       </c>
@@ -7800,7 +7800,7 @@
         <v>100000092629</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>3</v>
       </c>
@@ -7825,7 +7825,7 @@
       <c r="H12" s="9"/>
       <c r="I12" s="27"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>4</v>
       </c>
@@ -7854,7 +7854,7 @@
         <v>100000090079</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D14" s="20" t="s">
         <v>23</v>
       </c>
@@ -7874,7 +7874,7 @@
         <v>100000089571</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D15" s="9" t="s">
         <v>25</v>
       </c>
@@ -7894,7 +7894,7 @@
         <v>100000089370</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>5</v>
       </c>
@@ -7917,7 +7917,7 @@
         <v>100000091786</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>6</v>
       </c>
@@ -7946,7 +7946,7 @@
         <v>100000091343</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D18" s="34" t="s">
         <v>95</v>
       </c>
@@ -7966,7 +7966,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D19" s="19" t="s">
         <v>101</v>
       </c>
@@ -7986,7 +7986,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>7</v>
       </c>
@@ -8015,7 +8015,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D21" s="3" t="s">
         <v>193</v>
       </c>
@@ -8035,7 +8035,7 @@
         <v>100000085918</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>8</v>
       </c>
@@ -8064,7 +8064,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D23" s="41" t="s">
         <v>116</v>
       </c>
@@ -8084,7 +8084,7 @@
         <v>100000093039</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>9</v>
       </c>
@@ -8113,7 +8113,7 @@
         <v>100000090564</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>10</v>
       </c>
@@ -8142,7 +8142,7 @@
         <v>100000093061</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>11</v>
       </c>
@@ -8165,7 +8165,7 @@
         <v>100000085460</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>12</v>
       </c>
@@ -8194,7 +8194,7 @@
         <v>100000084795</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>13</v>
       </c>
@@ -8217,7 +8217,7 @@
         <v>100000092375</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>14</v>
       </c>
@@ -8240,7 +8240,7 @@
         <v>100000091721</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>15</v>
       </c>
@@ -8263,7 +8263,7 @@
         <v>100000091518</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>16</v>
       </c>
@@ -8286,7 +8286,7 @@
         <v>100000090229</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>17</v>
       </c>
@@ -8309,7 +8309,7 @@
         <v>100000090270</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>18</v>
       </c>
@@ -8332,7 +8332,7 @@
         <v>100000092362</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>19</v>
       </c>
@@ -8361,7 +8361,7 @@
         <v>100000090494</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D35" s="3" t="s">
         <v>211</v>
       </c>
@@ -8381,7 +8381,7 @@
         <v>100000076239</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D36" s="3" t="s">
         <v>216</v>
       </c>
@@ -8401,7 +8401,7 @@
         <v>100000076257</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>20</v>
       </c>
@@ -8430,7 +8430,7 @@
         <v>100000090152</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>21</v>
       </c>
@@ -8459,7 +8459,7 @@
         <v>100000092550</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D39" s="3" t="s">
         <v>239</v>
       </c>
@@ -8479,7 +8479,7 @@
         <v>100000086711</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D40" s="3" t="s">
         <v>244</v>
       </c>
@@ -8499,7 +8499,7 @@
         <v>100000092260</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D41" s="3" t="s">
         <v>249</v>
       </c>
@@ -8519,7 +8519,7 @@
         <v>100000085172</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D42" s="3" t="s">
         <v>254</v>
       </c>
@@ -8539,7 +8539,7 @@
         <v>100000084215</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D43" s="3" t="s">
         <v>479</v>
       </c>
@@ -8559,7 +8559,7 @@
         <v>100000085172</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D44" s="3" t="s">
         <v>264</v>
       </c>
@@ -8579,7 +8579,7 @@
         <v>100000086187</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D45" s="3" t="s">
         <v>269</v>
       </c>
@@ -8599,7 +8599,7 @@
         <v>100000086691</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>22</v>
       </c>
@@ -8628,7 +8628,7 @@
         <v>100000139489</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>23</v>
       </c>
@@ -8657,7 +8657,7 @@
         <v>100000128434</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D48" s="3" t="s">
         <v>295</v>
       </c>
@@ -8677,7 +8677,7 @@
         <v>100000174462</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>24</v>
       </c>
@@ -8702,7 +8702,7 @@
       <c r="H49" s="84"/>
       <c r="I49" s="84"/>
     </row>
-    <row r="50" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>25</v>
       </c>
@@ -8731,7 +8731,7 @@
         <v>100000090503</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>26</v>
       </c>
@@ -8760,7 +8760,7 @@
         <v>100000091366</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D52" s="37" t="s">
         <v>483</v>
       </c>
@@ -8780,7 +8780,7 @@
         <v>100000091840</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>27</v>
       </c>
@@ -8809,7 +8809,7 @@
         <v>100000088816</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D54" s="3" t="s">
         <v>484</v>
       </c>
@@ -8829,7 +8829,7 @@
         <v>100000091602</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D55" s="3" t="s">
         <v>351</v>
       </c>
@@ -8849,7 +8849,7 @@
         <v>100000130680</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D56" s="3" t="s">
         <v>354</v>
       </c>
@@ -8869,7 +8869,7 @@
         <v>100000141420</v>
       </c>
     </row>
-    <row r="57" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>28</v>
       </c>
@@ -8898,7 +8898,7 @@
         <v>100000093275</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>29</v>
       </c>
@@ -8921,7 +8921,7 @@
         <v>100000092121</v>
       </c>
     </row>
-    <row r="59" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>30</v>
       </c>
@@ -8944,7 +8944,7 @@
         <v>100000091697</v>
       </c>
     </row>
-    <row r="60" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>31</v>
       </c>
@@ -8973,7 +8973,7 @@
         <v>100000086673</v>
       </c>
     </row>
-    <row r="61" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>32</v>
       </c>
@@ -8993,7 +8993,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>33</v>
       </c>
@@ -9022,7 +9022,7 @@
         <v>100000092628</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D63" s="3" t="s">
         <v>406</v>
       </c>
@@ -9042,7 +9042,7 @@
         <v>100000090551</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D64" s="37" t="s">
         <v>411</v>
       </c>
@@ -9062,7 +9062,7 @@
         <v>100000084735</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D65" s="37" t="s">
         <v>416</v>
       </c>
@@ -9082,7 +9082,7 @@
         <v>100000129152</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>34</v>
       </c>
@@ -9105,7 +9105,7 @@
         <v>100000092074</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>35</v>
       </c>
@@ -9134,7 +9134,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D68" s="37" t="s">
         <v>468</v>
       </c>
@@ -9154,7 +9154,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>36</v>
       </c>
@@ -9183,7 +9183,7 @@
         <v>100000085009</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D70" s="37" t="s">
         <v>447</v>
       </c>
@@ -9203,7 +9203,7 @@
         <v>100000090111</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>37</v>
       </c>
@@ -9232,12 +9232,12 @@
         <v>100000115886</v>
       </c>
     </row>
-    <row r="74" spans="1:9" ht="21" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A74" s="89" t="s">
         <v>530</v>
       </c>
     </row>
-    <row r="77" spans="1:9" ht="96.6" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A77" s="85"/>
       <c r="B77" s="86" t="s">
         <v>520</v>
@@ -9252,7 +9252,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>1</v>
       </c>
@@ -9269,7 +9269,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D79" s="9" t="s">
         <v>11</v>
       </c>
@@ -9277,7 +9277,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D80" s="9" t="s">
         <v>478</v>
       </c>
@@ -9285,7 +9285,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D81" s="9" t="s">
         <v>14</v>
       </c>
@@ -9293,7 +9293,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>2</v>
       </c>
@@ -9310,7 +9310,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D83" s="9" t="s">
         <v>18</v>
       </c>
@@ -9318,7 +9318,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>3</v>
       </c>
@@ -9335,7 +9335,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>4</v>
       </c>
@@ -9352,7 +9352,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D86" s="20" t="s">
         <v>23</v>
       </c>
@@ -9360,7 +9360,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D87" s="9" t="s">
         <v>25</v>
       </c>
@@ -9368,7 +9368,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>5</v>
       </c>
@@ -9385,7 +9385,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>6</v>
       </c>
@@ -9402,7 +9402,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D90" s="34" t="s">
         <v>95</v>
       </c>
@@ -9410,7 +9410,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D91" s="19" t="s">
         <v>101</v>
       </c>
@@ -9418,7 +9418,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>7</v>
       </c>
@@ -9435,7 +9435,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D93" s="3" t="s">
         <v>193</v>
       </c>
@@ -9443,7 +9443,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>8</v>
       </c>
@@ -9460,7 +9460,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D95" s="41" t="s">
         <v>116</v>
       </c>
@@ -9468,7 +9468,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>9</v>
       </c>
@@ -9485,7 +9485,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>10</v>
       </c>
@@ -9502,7 +9502,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="98" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>11</v>
       </c>
@@ -9519,7 +9519,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>12</v>
       </c>
@@ -9536,7 +9536,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>13</v>
       </c>
@@ -9553,7 +9553,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>14</v>
       </c>
@@ -9570,7 +9570,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>15</v>
       </c>
@@ -9587,7 +9587,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>16</v>
       </c>
@@ -9604,7 +9604,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="104" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>17</v>
       </c>
@@ -9621,7 +9621,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="105" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>18</v>
       </c>
@@ -9638,7 +9638,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>19</v>
       </c>
@@ -9655,7 +9655,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D107" s="3" t="s">
         <v>211</v>
       </c>
@@ -9663,7 +9663,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D108" s="3" t="s">
         <v>216</v>
       </c>
@@ -9671,7 +9671,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>20</v>
       </c>
@@ -9688,7 +9688,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>21</v>
       </c>
@@ -9705,7 +9705,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D111" s="3" t="s">
         <v>239</v>
       </c>
@@ -9713,7 +9713,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D112" s="3" t="s">
         <v>244</v>
       </c>
@@ -9721,7 +9721,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D113" s="3" t="s">
         <v>249</v>
       </c>
@@ -9729,7 +9729,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D114" s="3" t="s">
         <v>254</v>
       </c>
@@ -9737,7 +9737,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D115" s="3" t="s">
         <v>479</v>
       </c>
@@ -9745,7 +9745,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D116" s="3" t="s">
         <v>264</v>
       </c>
@@ -9753,7 +9753,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D117" s="3" t="s">
         <v>269</v>
       </c>
@@ -9761,7 +9761,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>22</v>
       </c>
@@ -9778,7 +9778,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="119" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>23</v>
       </c>
@@ -9795,7 +9795,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D120" s="3" t="s">
         <v>295</v>
       </c>
@@ -9803,7 +9803,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="121" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>24</v>
       </c>
@@ -9820,7 +9820,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="122" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>25</v>
       </c>
@@ -9837,7 +9837,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>26</v>
       </c>
@@ -9854,7 +9854,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D124" s="37" t="s">
         <v>483</v>
       </c>
@@ -9862,7 +9862,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>27</v>
       </c>
@@ -9879,7 +9879,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D126" s="3" t="s">
         <v>484</v>
       </c>
@@ -9887,7 +9887,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D127" s="3" t="s">
         <v>351</v>
       </c>
@@ -9895,7 +9895,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D128" s="3" t="s">
         <v>354</v>
       </c>
@@ -9903,7 +9903,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="129" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>28</v>
       </c>
@@ -9920,7 +9920,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="130" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>29</v>
       </c>
@@ -9937,7 +9937,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="131" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>30</v>
       </c>
@@ -9954,7 +9954,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="132" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>31</v>
       </c>
@@ -9971,7 +9971,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="133" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>32</v>
       </c>
@@ -9985,7 +9985,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>33</v>
       </c>
@@ -10002,7 +10002,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D135" s="3" t="s">
         <v>406</v>
       </c>
@@ -10010,7 +10010,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D136" s="37" t="s">
         <v>411</v>
       </c>
@@ -10018,7 +10018,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D137" s="37" t="s">
         <v>416</v>
       </c>
@@ -10026,7 +10026,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>34</v>
       </c>
@@ -10043,7 +10043,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>35</v>
       </c>
@@ -10060,7 +10060,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D140" s="37" t="s">
         <v>468</v>
       </c>
@@ -10068,7 +10068,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>36</v>
       </c>
@@ -10085,7 +10085,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D142" s="37" t="s">
         <v>447</v>
       </c>
@@ -10093,7 +10093,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>37</v>
       </c>

</xml_diff>